<commit_message>
ode changes. Regularity ode complete.
</commit_message>
<xml_diff>
--- a/teaching/10550/section-1/10550-1.xlsx
+++ b/teaching/10550/section-1/10550-1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="85">
   <si>
     <t>Last Name</t>
   </si>
@@ -257,6 +257,30 @@
   </si>
   <si>
     <t>W1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sturdifen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jasmine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -631,15 +655,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -658,8 +682,14 @@
       <c r="H1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -673,7 +703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -692,8 +722,14 @@
       <c r="H3">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -712,8 +748,14 @@
       <c r="H4">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -732,8 +774,14 @@
       <c r="H5">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -752,8 +800,14 @@
       <c r="H6">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -772,8 +826,14 @@
       <c r="H7">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -792,8 +852,14 @@
       <c r="H8">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -812,8 +878,14 @@
       <c r="H9">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -832,8 +904,14 @@
       <c r="H10">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -852,8 +930,14 @@
       <c r="H11">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -872,8 +956,14 @@
       <c r="H12">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12">
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -892,8 +982,14 @@
       <c r="H13">
         <v>48</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -912,8 +1008,14 @@
       <c r="H14">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -932,8 +1034,14 @@
       <c r="H15">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -952,8 +1060,14 @@
       <c r="H16">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -972,8 +1086,14 @@
       <c r="H17">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -992,8 +1112,14 @@
       <c r="H18">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -1012,8 +1138,14 @@
       <c r="H19">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19">
+        <v>4</v>
+      </c>
+      <c r="J19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -1032,8 +1164,14 @@
       <c r="H20">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20">
+        <v>4</v>
+      </c>
+      <c r="J20">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>62</v>
       </c>
@@ -1052,8 +1190,14 @@
       <c r="H21">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -1072,8 +1216,14 @@
       <c r="H22">
         <v>50</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>68</v>
       </c>
@@ -1092,51 +1242,89 @@
       <c r="H23">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23">
+        <v>4</v>
+      </c>
+      <c r="J23">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" t="s">
+        <v>82</v>
+      </c>
+      <c r="G24" t="s">
+        <v>83</v>
+      </c>
+      <c r="H24" t="s">
+        <v>84</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
         <v>71</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>72</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>73</v>
       </c>
-      <c r="D24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24">
-        <v>4</v>
-      </c>
-      <c r="H24">
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="s">
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="J25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
         <v>74</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>75</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>76</v>
       </c>
-      <c r="D25" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25">
-        <v>4</v>
-      </c>
-      <c r="H25">
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26">
         <v>45</v>
       </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Finished burgers optimality. Needs polish
</commit_message>
<xml_diff>
--- a/teaching/10550/section-1/10550-1.xlsx
+++ b/teaching/10550/section-1/10550-1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="13580" tabRatio="500"/>
+    <workbookView xWindow="-280" yWindow="1280" windowWidth="21600" windowHeight="13580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="10550-1.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="83">
   <si>
     <t>Last Name</t>
   </si>
@@ -31,18 +31,6 @@
   </si>
   <si>
     <t>Role</t>
-  </si>
-  <si>
-    <t>Borelli</t>
-  </si>
-  <si>
-    <t>Mario</t>
-  </si>
-  <si>
-    <t>mario</t>
-  </si>
-  <si>
-    <t>Section Designer, Section Instructor</t>
   </si>
   <si>
     <t>Brucker</t>
@@ -281,6 +269,14 @@
   </si>
   <si>
     <t>?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -655,15 +651,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -677,19 +673,25 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>76</v>
+      </c>
+      <c r="K1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -702,8 +704,26 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>50</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>50</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -714,163 +734,199 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>44</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>50</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>50</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-      <c r="J3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>50</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>50</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>45</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>47</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>50</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>50</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>50</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>37</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
         <v>44</v>
       </c>
-      <c r="I4">
-        <v>4</v>
-      </c>
-      <c r="J4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5">
-        <v>50</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-      <c r="J5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <v>45</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="J6">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
-      <c r="H7">
-        <v>50</v>
-      </c>
-      <c r="I7">
-        <v>4</v>
-      </c>
-      <c r="J7">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>48</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
         <v>26</v>
       </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8">
-        <v>4</v>
-      </c>
-      <c r="H8">
-        <v>50</v>
-      </c>
-      <c r="I8">
-        <v>4</v>
-      </c>
-      <c r="J8">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G9">
         <v>4</v>
@@ -882,157 +938,193 @@
         <v>4</v>
       </c>
       <c r="J9">
+        <v>47</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <v>50</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>50</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>44</v>
+      </c>
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11">
+        <v>50</v>
+      </c>
+      <c r="K11">
+        <v>4</v>
+      </c>
+      <c r="L11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10">
-        <v>4</v>
-      </c>
-      <c r="H10">
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>50</v>
+      </c>
+      <c r="K12">
+        <v>4</v>
+      </c>
+      <c r="L12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>38</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <v>50</v>
+      </c>
+      <c r="K13">
+        <v>4</v>
+      </c>
+      <c r="L13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <v>48</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <v>47</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+      <c r="L14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
         <v>44</v>
       </c>
-      <c r="I10">
-        <v>4</v>
-      </c>
-      <c r="J10">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11">
-        <v>4</v>
-      </c>
-      <c r="H11">
-        <v>50</v>
-      </c>
-      <c r="I11">
-        <v>4</v>
-      </c>
-      <c r="J11">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12">
-        <v>4</v>
-      </c>
-      <c r="H12">
-        <v>44</v>
-      </c>
-      <c r="I12">
-        <v>4</v>
-      </c>
-      <c r="J12">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13">
-        <v>4</v>
-      </c>
-      <c r="H13">
-        <v>48</v>
-      </c>
-      <c r="I13">
-        <v>2</v>
-      </c>
-      <c r="J13">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14">
-        <v>2</v>
-      </c>
-      <c r="H14">
-        <v>38</v>
-      </c>
-      <c r="I14">
-        <v>4</v>
-      </c>
-      <c r="J14">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>45</v>
       </c>
-      <c r="C15" t="s">
-        <v>46</v>
-      </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G15">
         <v>4</v>
       </c>
       <c r="H15">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I15">
         <v>4</v>
@@ -1040,123 +1132,153 @@
       <c r="J15">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15">
+        <v>4</v>
+      </c>
+      <c r="L15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
         <v>47</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>48</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16">
+        <v>48</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>50</v>
+      </c>
+      <c r="K16">
+        <v>4</v>
+      </c>
+      <c r="L16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
         <v>49</v>
       </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16">
-        <v>4</v>
-      </c>
-      <c r="H16">
-        <v>45</v>
-      </c>
-      <c r="I16">
-        <v>4</v>
-      </c>
-      <c r="J16">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" t="s">
-        <v>50</v>
-      </c>
       <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
         <v>51</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>50</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>50</v>
+      </c>
+      <c r="K17">
+        <v>4</v>
+      </c>
+      <c r="L17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
         <v>52</v>
       </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17">
-        <v>4</v>
-      </c>
-      <c r="H17">
-        <v>48</v>
-      </c>
-      <c r="I17">
-        <v>4</v>
-      </c>
-      <c r="J17">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>53</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>54</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18">
+        <v>50</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <v>50</v>
+      </c>
+      <c r="K18">
+        <v>4</v>
+      </c>
+      <c r="L18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
         <v>55</v>
       </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18">
-        <v>4</v>
-      </c>
-      <c r="H18">
-        <v>50</v>
-      </c>
-      <c r="I18">
-        <v>4</v>
-      </c>
-      <c r="J18">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>56</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>57</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19">
+        <v>38</v>
+      </c>
+      <c r="I19">
+        <v>4</v>
+      </c>
+      <c r="J19">
+        <v>50</v>
+      </c>
+      <c r="K19">
+        <v>4</v>
+      </c>
+      <c r="L19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
         <v>58</v>
       </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19">
-        <v>4</v>
-      </c>
-      <c r="H19">
-        <v>50</v>
-      </c>
-      <c r="I19">
-        <v>4</v>
-      </c>
-      <c r="J19">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>59</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>60</v>
       </c>
-      <c r="C20" t="s">
-        <v>61</v>
-      </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G20">
         <v>4</v>
@@ -1165,30 +1287,36 @@
         <v>38</v>
       </c>
       <c r="I20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J20">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+        <v>50</v>
+      </c>
+      <c r="K20">
+        <v>4</v>
+      </c>
+      <c r="L20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
         <v>62</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>63</v>
       </c>
-      <c r="C21" t="s">
-        <v>64</v>
-      </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G21">
         <v>4</v>
       </c>
       <c r="H21">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="I21">
         <v>2</v>
@@ -1196,129 +1324,133 @@
       <c r="J21">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21">
+        <v>4</v>
+      </c>
+      <c r="L21">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" t="s">
         <v>65</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>66</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
+      <c r="H22">
+        <v>38</v>
+      </c>
+      <c r="I22">
+        <v>4</v>
+      </c>
+      <c r="J22">
+        <v>47</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+      <c r="L22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" t="s">
+        <v>79</v>
+      </c>
+      <c r="H23" t="s">
+        <v>80</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>50</v>
+      </c>
+      <c r="K23">
+        <v>4</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" t="s">
         <v>67</v>
       </c>
-      <c r="D22" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22">
-        <v>4</v>
-      </c>
-      <c r="H22">
-        <v>50</v>
-      </c>
-      <c r="I22">
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24">
+        <v>4</v>
+      </c>
+      <c r="H24">
+        <v>48</v>
+      </c>
+      <c r="I24">
         <v>2</v>
       </c>
-      <c r="J22">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="J24">
+        <v>50</v>
+      </c>
+      <c r="K24">
+        <v>2</v>
+      </c>
+      <c r="L24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
         <v>70</v>
       </c>
-      <c r="D23" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23">
-        <v>4</v>
-      </c>
-      <c r="H23">
-        <v>38</v>
-      </c>
-      <c r="I23">
-        <v>4</v>
-      </c>
-      <c r="J23">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B24" t="s">
-        <v>82</v>
-      </c>
-      <c r="G24" t="s">
-        <v>83</v>
-      </c>
-      <c r="H24" t="s">
-        <v>84</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>71</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>72</v>
       </c>
-      <c r="C25" t="s">
-        <v>73</v>
-      </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G25">
         <v>4</v>
       </c>
       <c r="H25">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I25">
         <v>2</v>
       </c>
       <c r="J25">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26">
-        <v>4</v>
-      </c>
-      <c r="H26">
-        <v>45</v>
-      </c>
-      <c r="I26">
-        <v>2</v>
-      </c>
-      <c r="J26">
         <v>47</v>
+      </c>
+      <c r="K25">
+        <v>4</v>
+      </c>
+      <c r="L25">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hr holder done with picard iteration proof
</commit_message>
<xml_diff>
--- a/teaching/10550/section-1/10550-1.xlsx
+++ b/teaching/10550/section-1/10550-1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-280" yWindow="1280" windowWidth="21600" windowHeight="13580" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="20480" windowHeight="14740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="10550-1.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="85">
   <si>
     <t>Last Name</t>
   </si>
@@ -277,6 +277,14 @@
   </si>
   <si>
     <t>W3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -654,7 +662,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="E1" sqref="E1:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -672,23 +680,29 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
+        <v>74</v>
+      </c>
       <c r="G1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="J1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="K1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="L1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -704,6 +718,12 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>50</v>
+      </c>
       <c r="G2">
         <v>4</v>
       </c>
@@ -720,7 +740,7 @@
         <v>4</v>
       </c>
       <c r="L2">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -736,20 +756,26 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>44</v>
+      </c>
       <c r="G3">
         <v>4</v>
       </c>
       <c r="H3">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J3">
         <v>50</v>
       </c>
       <c r="K3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L3">
         <v>50</v>
@@ -768,6 +794,12 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
       <c r="G4">
         <v>4</v>
       </c>
@@ -781,10 +813,10 @@
         <v>50</v>
       </c>
       <c r="K4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L4">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -800,17 +832,23 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>45</v>
+      </c>
       <c r="G5">
         <v>4</v>
       </c>
       <c r="H5">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I5">
         <v>4</v>
       </c>
       <c r="J5">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K5">
         <v>4</v>
@@ -832,6 +870,12 @@
       <c r="D6" t="s">
         <v>7</v>
       </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
       <c r="G6">
         <v>4</v>
       </c>
@@ -842,13 +886,13 @@
         <v>4</v>
       </c>
       <c r="J6">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -864,17 +908,23 @@
       <c r="D7" t="s">
         <v>7</v>
       </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>50</v>
+      </c>
       <c r="G7">
         <v>4</v>
       </c>
       <c r="H7">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="I7">
         <v>4</v>
       </c>
       <c r="J7">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="K7">
         <v>4</v>
@@ -896,23 +946,29 @@
       <c r="D8" t="s">
         <v>7</v>
       </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>44</v>
+      </c>
       <c r="G8">
         <v>4</v>
       </c>
       <c r="H8">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="I8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J8">
+        <v>50</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
         <v>48</v>
-      </c>
-      <c r="K8">
-        <v>2</v>
-      </c>
-      <c r="L8">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -928,23 +984,29 @@
       <c r="D9" t="s">
         <v>7</v>
       </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>44</v>
+      </c>
       <c r="G9">
         <v>4</v>
       </c>
       <c r="H9">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J9">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K9">
         <v>2</v>
       </c>
       <c r="L9">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -960,6 +1022,12 @@
       <c r="D10" t="s">
         <v>7</v>
       </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>50</v>
+      </c>
       <c r="G10">
         <v>4</v>
       </c>
@@ -967,16 +1035,16 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J10">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="K10">
         <v>2</v>
       </c>
       <c r="L10">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -992,23 +1060,29 @@
       <c r="D11" t="s">
         <v>7</v>
       </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>44</v>
+      </c>
       <c r="G11">
         <v>4</v>
       </c>
       <c r="H11">
+        <v>50</v>
+      </c>
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11">
+        <v>50</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
         <v>44</v>
-      </c>
-      <c r="I11">
-        <v>4</v>
-      </c>
-      <c r="J11">
-        <v>50</v>
-      </c>
-      <c r="K11">
-        <v>4</v>
-      </c>
-      <c r="L11">
-        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1024,23 +1098,29 @@
       <c r="D12" t="s">
         <v>7</v>
       </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>48</v>
+      </c>
       <c r="G12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H12">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J12">
         <v>50</v>
       </c>
       <c r="K12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L12">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1056,11 +1136,17 @@
       <c r="D13" t="s">
         <v>7</v>
       </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>38</v>
+      </c>
       <c r="G13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H13">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="I13">
         <v>4</v>
@@ -1069,10 +1155,10 @@
         <v>50</v>
       </c>
       <c r="K13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L13">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1088,20 +1174,26 @@
       <c r="D14" t="s">
         <v>7</v>
       </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <v>48</v>
+      </c>
       <c r="G14">
         <v>4</v>
       </c>
       <c r="H14">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I14">
         <v>4</v>
       </c>
       <c r="J14">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L14">
         <v>50</v>
@@ -1120,17 +1212,23 @@
       <c r="D15" t="s">
         <v>7</v>
       </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>45</v>
+      </c>
       <c r="G15">
         <v>4</v>
       </c>
       <c r="H15">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I15">
         <v>4</v>
       </c>
       <c r="J15">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K15">
         <v>4</v>
@@ -1152,23 +1250,29 @@
       <c r="D16" t="s">
         <v>7</v>
       </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>48</v>
+      </c>
       <c r="G16">
         <v>4</v>
       </c>
       <c r="H16">
+        <v>50</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>50</v>
+      </c>
+      <c r="K16">
+        <v>4</v>
+      </c>
+      <c r="L16">
         <v>48</v>
-      </c>
-      <c r="I16">
-        <v>4</v>
-      </c>
-      <c r="J16">
-        <v>50</v>
-      </c>
-      <c r="K16">
-        <v>4</v>
-      </c>
-      <c r="L16">
-        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1184,6 +1288,12 @@
       <c r="D17" t="s">
         <v>7</v>
       </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>50</v>
+      </c>
       <c r="G17">
         <v>4</v>
       </c>
@@ -1216,6 +1326,12 @@
       <c r="D18" t="s">
         <v>7</v>
       </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>50</v>
+      </c>
       <c r="G18">
         <v>4</v>
       </c>
@@ -1248,11 +1364,17 @@
       <c r="D19" t="s">
         <v>7</v>
       </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>38</v>
+      </c>
       <c r="G19">
         <v>4</v>
       </c>
       <c r="H19">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="I19">
         <v>4</v>
@@ -1264,7 +1386,7 @@
         <v>4</v>
       </c>
       <c r="L19">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1280,14 +1402,20 @@
       <c r="D20" t="s">
         <v>7</v>
       </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>38</v>
+      </c>
       <c r="G20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H20">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="I20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J20">
         <v>50</v>
@@ -1296,7 +1424,7 @@
         <v>4</v>
       </c>
       <c r="L20">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1312,23 +1440,29 @@
       <c r="D21" t="s">
         <v>7</v>
       </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>50</v>
+      </c>
       <c r="G21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H21">
         <v>50</v>
       </c>
       <c r="I21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J21">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="K21">
         <v>4</v>
       </c>
       <c r="L21">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1344,23 +1478,29 @@
       <c r="D22" t="s">
         <v>7</v>
       </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>38</v>
+      </c>
       <c r="G22">
         <v>4</v>
       </c>
       <c r="H22">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="I22">
         <v>4</v>
       </c>
       <c r="J22">
+        <v>50</v>
+      </c>
+      <c r="K22">
+        <v>2</v>
+      </c>
+      <c r="L22">
         <v>47</v>
-      </c>
-      <c r="K22">
-        <v>4</v>
-      </c>
-      <c r="L22">
-        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1370,20 +1510,26 @@
       <c r="B23" t="s">
         <v>78</v>
       </c>
-      <c r="G23" t="s">
+      <c r="E23" t="s">
         <v>79</v>
       </c>
-      <c r="H23" t="s">
+      <c r="F23" t="s">
         <v>80</v>
       </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>50</v>
+      </c>
       <c r="I23">
+        <v>4</v>
+      </c>
+      <c r="J23">
         <v>0</v>
       </c>
-      <c r="J23">
-        <v>50</v>
-      </c>
       <c r="K23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -1402,23 +1548,29 @@
       <c r="D24" t="s">
         <v>7</v>
       </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>48</v>
+      </c>
       <c r="G24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H24">
+        <v>50</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+      <c r="J24">
+        <v>50</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
         <v>48</v>
-      </c>
-      <c r="I24">
-        <v>2</v>
-      </c>
-      <c r="J24">
-        <v>50</v>
-      </c>
-      <c r="K24">
-        <v>2</v>
-      </c>
-      <c r="L24">
-        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1434,17 +1586,23 @@
       <c r="D25" t="s">
         <v>7</v>
       </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+      <c r="F25">
+        <v>45</v>
+      </c>
       <c r="G25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H25">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J25">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K25">
         <v>4</v>
@@ -1454,6 +1612,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
cv changes, thesis changes--holder now has polished burgers argument
</commit_message>
<xml_diff>
--- a/teaching/10550/section-1/10550-1.xlsx
+++ b/teaching/10550/section-1/10550-1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="20480" windowHeight="14740" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="25540" windowHeight="14600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="10550-1.csv" sheetId="1" r:id="rId1"/>
@@ -264,14 +264,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Q3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -285,6 +277,14 @@
   </si>
   <si>
     <t>W4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -292,12 +292,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10"/>
@@ -659,15 +653,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E25"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -693,19 +687,25 @@
         <v>76</v>
       </c>
       <c r="I1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" t="s">
         <v>81</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>82</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>83</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -742,8 +742,14 @@
       <c r="L2">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -780,8 +786,14 @@
       <c r="L3">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -818,8 +830,14 @@
       <c r="L4">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4">
+        <v>4</v>
+      </c>
+      <c r="N4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -856,8 +874,14 @@
       <c r="L5">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -894,8 +918,14 @@
       <c r="L6">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -932,8 +962,14 @@
       <c r="L7">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -970,8 +1006,14 @@
       <c r="L8">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1008,8 +1050,14 @@
       <c r="L9">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9">
+        <v>4</v>
+      </c>
+      <c r="N9">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1046,8 +1094,14 @@
       <c r="L10">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="N10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1084,8 +1138,14 @@
       <c r="L11">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1122,8 +1182,14 @@
       <c r="L12">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12">
+        <v>4</v>
+      </c>
+      <c r="N12">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1160,8 +1226,14 @@
       <c r="L13">
         <v>47</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13">
+        <v>2</v>
+      </c>
+      <c r="N13">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1198,8 +1270,14 @@
       <c r="L14">
         <v>50</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14">
+        <v>4</v>
+      </c>
+      <c r="N14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1236,8 +1314,14 @@
       <c r="L15">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -1274,8 +1358,14 @@
       <c r="L16">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1312,8 +1402,14 @@
       <c r="L17">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17">
+        <v>2</v>
+      </c>
+      <c r="N17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -1350,8 +1446,14 @@
       <c r="L18">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18">
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1388,8 +1490,14 @@
       <c r="L19">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19">
+        <v>4</v>
+      </c>
+      <c r="N19">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1426,8 +1534,14 @@
       <c r="L20">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -1464,8 +1578,14 @@
       <c r="L21">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21">
+        <v>2</v>
+      </c>
+      <c r="N21">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -1502,19 +1622,25 @@
       <c r="L22">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22">
+        <v>2</v>
+      </c>
+      <c r="N22">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>77</v>
       </c>
       <c r="B23" t="s">
         <v>78</v>
       </c>
-      <c r="E23" t="s">
-        <v>79</v>
-      </c>
-      <c r="F23" t="s">
-        <v>80</v>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>48</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -1534,8 +1660,14 @@
       <c r="L23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="M23">
+        <v>4</v>
+      </c>
+      <c r="N23">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>67</v>
       </c>
@@ -1572,8 +1704,14 @@
       <c r="L24">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
         <v>70</v>
       </c>
@@ -1610,12 +1748,16 @@
       <c r="L25">
         <v>50</v>
       </c>
+      <c r="M25">
+        <v>2</v>
+      </c>
+      <c r="N25">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
thesis mass edits. created hr holder beamer presentation
</commit_message>
<xml_diff>
--- a/teaching/10550/section-1/10550-1.xlsx
+++ b/teaching/10550/section-1/10550-1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="25540" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="20480" windowHeight="14740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="10550-1.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="89">
   <si>
     <t>Last Name</t>
   </si>
@@ -285,6 +285,22 @@
   </si>
   <si>
     <t>W5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q7</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -292,6 +308,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10"/>
@@ -653,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1755,9 +1777,657 @@
         <v>45</v>
       </c>
     </row>
+    <row r="29" spans="1:14">
+      <c r="E29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F29" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" t="s">
+        <v>88</v>
+      </c>
+      <c r="H29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <v>47</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="H31">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>35</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>38</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
+        <v>43</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36">
+        <v>43</v>
+      </c>
+      <c r="G36">
+        <v>2</v>
+      </c>
+      <c r="H36">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37">
+        <v>4</v>
+      </c>
+      <c r="F37">
+        <v>43</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
+      </c>
+      <c r="H37">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38">
+        <v>4</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>4</v>
+      </c>
+      <c r="H38">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <v>35</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="F41">
+        <v>40</v>
+      </c>
+      <c r="G41">
+        <v>2</v>
+      </c>
+      <c r="H41">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <v>44</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+      <c r="H42">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43">
+        <v>43</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <v>43</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="H44">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45">
+        <v>4</v>
+      </c>
+      <c r="F45">
+        <v>40</v>
+      </c>
+      <c r="G45">
+        <v>2</v>
+      </c>
+      <c r="H45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46">
+        <v>4</v>
+      </c>
+      <c r="F46">
+        <v>47</v>
+      </c>
+      <c r="G46">
+        <v>2</v>
+      </c>
+      <c r="H46">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47">
+        <v>4</v>
+      </c>
+      <c r="F47">
+        <v>47</v>
+      </c>
+      <c r="G47">
+        <v>2</v>
+      </c>
+      <c r="H47">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" t="s">
+        <v>57</v>
+      </c>
+      <c r="D48" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48">
+        <v>44</v>
+      </c>
+      <c r="G48">
+        <v>2</v>
+      </c>
+      <c r="H48">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" t="s">
+        <v>60</v>
+      </c>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49">
+        <v>4</v>
+      </c>
+      <c r="F49">
+        <v>44</v>
+      </c>
+      <c r="G49">
+        <v>4</v>
+      </c>
+      <c r="H49">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <v>35</v>
+      </c>
+      <c r="G50">
+        <v>2</v>
+      </c>
+      <c r="H50">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" t="s">
+        <v>66</v>
+      </c>
+      <c r="D51" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>44</v>
+      </c>
+      <c r="G51">
+        <v>4</v>
+      </c>
+      <c r="H51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>77</v>
+      </c>
+      <c r="B52" t="s">
+        <v>78</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52">
+        <v>35</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53" t="s">
+        <v>69</v>
+      </c>
+      <c r="D53" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53">
+        <v>4</v>
+      </c>
+      <c r="F53">
+        <v>40</v>
+      </c>
+      <c r="G53">
+        <v>4</v>
+      </c>
+      <c r="H53">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" t="s">
+        <v>72</v>
+      </c>
+      <c r="D54" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54">
+        <v>43</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+      <c r="H54">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>